<commit_message>
Actualizando lista de Pendientes...
</commit_message>
<xml_diff>
--- a/cosas_faltantes/2019/Faltantes.xlsx
+++ b/cosas_faltantes/2019/Faltantes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>PUNCH LIST 2019</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>Fecha Finalización</t>
+  </si>
+  <si>
+    <t>Leer configuracion para cargar la EDU-CIAA con la informacion que corresponda.</t>
+  </si>
+  <si>
+    <t>Hacer que funcionen la ida y la vuelta al mismo tiempo.</t>
+  </si>
+  <si>
+    <t>No se va a hacer</t>
+  </si>
+  <si>
+    <t>FINALIZADO</t>
+  </si>
+  <si>
+    <t>No se va a hacer.</t>
   </si>
 </sst>
 </file>
@@ -131,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -262,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,15 +300,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -315,17 +327,28 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,34 +653,34 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:B12"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.28515625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="74.28515625" style="12" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" style="12" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -665,351 +688,375 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <v>0</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="23">
+      <c r="C4" s="9"/>
+      <c r="D4" s="17">
         <v>43518</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="14">
         <v>0</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="24">
+      <c r="C5" s="10"/>
+      <c r="D5" s="18">
         <v>43518</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>0</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="24">
+      <c r="C6" s="10"/>
+      <c r="D6" s="18">
         <v>43518</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="14">
         <v>0.85</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="18">
         <v>43511</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="14">
         <v>0</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="14">
         <v>0.2</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="13">
         <v>0</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="17">
+      <c r="C18" s="9"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="14">
+        <v>0.85</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="13">
         <v>0</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="14">
+        <v>0</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="13">
         <v>1</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="16">
+      <c r="C32" s="9"/>
+      <c r="D32" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="14">
+        <v>1</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="14">
         <v>0</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="17">
-        <v>0.85</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="16">
+      <c r="C34" s="10"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="14">
         <v>0</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="17">
-        <v>0</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="16">
-        <v>0</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="17">
-        <v>0</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="13"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="13"/>
+      <c r="C40" s="10"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="13"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="13"/>
+      <c r="C42" s="10"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="13"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="13"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A37:D37"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Subiendo cambios en cosas_faltantes.xml
</commit_message>
<xml_diff>
--- a/cosas_faltantes/2019/Faltantes.xlsx
+++ b/cosas_faltantes/2019/Faltantes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF21167-7333-42D8-BDC2-691DD9278B23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -120,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -329,26 +330,26 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,6 +359,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -406,7 +410,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,9 +443,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,6 +495,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -649,11 +687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -666,12 +704,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -688,12 +726,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -755,7 +793,7 @@
       <c r="C8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -777,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -789,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -830,12 +868,12 @@
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
@@ -882,12 +920,12 @@
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="23"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
@@ -909,7 +947,7 @@
       <c r="C26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -938,12 +976,12 @@
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -953,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="9"/>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -965,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="10"/>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="19" t="s">
         <v>31</v>
       </c>
     </row>
@@ -992,12 +1030,12 @@
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
@@ -1064,7 +1102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1076,7 +1114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>